<commit_message>
Scan profiles plot changed from Bn to bn
</commit_message>
<xml_diff>
--- a/WMM_All_configurations/MCBXFA_02_Inner_Iron_600_20220510/Roxie_vs_MM_NormalMCBXFA_02_Inner_Iron_600_20220510.xlsx
+++ b/WMM_All_configurations/MCBXFA_02_Inner_Iron_600_20220510/Roxie_vs_MM_NormalMCBXFA_02_Inner_Iron_600_20220510.xlsx
@@ -621,46 +621,46 @@
         <v>-0.2988425617549172</v>
       </c>
       <c r="S2">
-        <v>-9.727776421031244</v>
+        <v>0.0003374155165390692</v>
       </c>
       <c r="T2">
-        <v>-23.6164547842054</v>
+        <v>0.001337716227943058</v>
       </c>
       <c r="U2">
-        <v>0.07297155402910539</v>
+        <v>-3.836301416762852E-06</v>
       </c>
       <c r="V2">
-        <v>3.163732635147427</v>
+        <v>-7.935477442629211E-05</v>
       </c>
       <c r="W2">
-        <v>0.03455639280639029</v>
+        <v>-9.125363393711146E-07</v>
       </c>
       <c r="X2">
-        <v>-3.749163636960444</v>
+        <v>0.000103319795918088</v>
       </c>
       <c r="Y2">
-        <v>-0.03719803425637391</v>
+        <v>9.641793466235713E-07</v>
       </c>
       <c r="Z2">
-        <v>-1.430227016780397</v>
+        <v>3.042224649662914E-05</v>
       </c>
       <c r="AA2">
-        <v>0.004339350245012328</v>
+        <v>-2.557583858044626E-08</v>
       </c>
       <c r="AB2">
-        <v>-1.813934712341678</v>
+        <v>4.90838083535676E-05</v>
       </c>
       <c r="AC2">
-        <v>0.03295322185671454</v>
+        <v>-1.007132172838627E-06</v>
       </c>
       <c r="AD2">
-        <v>7.736624931039496</v>
+        <v>-0.0002135352256541946</v>
       </c>
       <c r="AE2">
-        <v>-0.02138943740816093</v>
+        <v>5.455179660721536E-07</v>
       </c>
       <c r="AF2">
-        <v>-4.668774128269343</v>
+        <v>0.0001170906689813567</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -719,46 +719,46 @@
         <v>3883.249378802444</v>
       </c>
       <c r="S3">
-        <v>-4.310146059960727</v>
+        <v>0.003145268273837382</v>
       </c>
       <c r="T3">
-        <v>-102.2295270416021</v>
+        <v>-5.159703901125607</v>
       </c>
       <c r="U3">
-        <v>0.2098808488041859</v>
+        <v>0.0002426066663963457</v>
       </c>
       <c r="V3">
-        <v>-41.24458552371551</v>
+        <v>-3.447569149519026</v>
       </c>
       <c r="W3">
-        <v>0.009078976583652964</v>
+        <v>-1.342709741750565E-05</v>
       </c>
       <c r="X3">
-        <v>-4.916793741932531</v>
+        <v>-3.807632378352325</v>
       </c>
       <c r="Y3">
-        <v>0.006673221595687773</v>
+        <v>1.803884600817608E-06</v>
       </c>
       <c r="Z3">
-        <v>-1.727976748465495</v>
+        <v>-0.7959591041396851</v>
       </c>
       <c r="AA3">
-        <v>0.002233848600394632</v>
+        <v>5.387616708110245E-07</v>
       </c>
       <c r="AB3">
-        <v>-0.5432594962308495</v>
+        <v>0.06023825116324097</v>
       </c>
       <c r="AC3">
-        <v>-0.004737495432041968</v>
+        <v>-1.362621105055171E-06</v>
       </c>
       <c r="AD3">
-        <v>-0.6079292103552552</v>
+        <v>-0.6113731744562918</v>
       </c>
       <c r="AE3">
-        <v>-0.004324656446714305</v>
+        <v>5.870551755424866E-07</v>
       </c>
       <c r="AF3">
-        <v>0.5943259143989457</v>
+        <v>0.01608037360569016</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -817,46 +817,46 @@
         <v>9999.846038205334</v>
       </c>
       <c r="S4">
-        <v>-0.001687942160930089</v>
+        <v>-0.001687946010371525</v>
       </c>
       <c r="T4">
-        <v>-13.02642160016146</v>
+        <v>-13.02621989082303</v>
       </c>
       <c r="U4">
-        <v>-0.0006945515308829109</v>
+        <v>-0.0006945508100858341</v>
       </c>
       <c r="V4">
-        <v>0.2950929602236564</v>
+        <v>0.2950884838163252</v>
       </c>
       <c r="W4">
-        <v>-4.51678998556056E-05</v>
+        <v>-4.516807969753136E-05</v>
       </c>
       <c r="X4">
-        <v>1.77631658288761</v>
+        <v>1.776289229535417</v>
       </c>
       <c r="Y4">
-        <v>3.556734129319337E-06</v>
+        <v>3.556611376828276E-06</v>
       </c>
       <c r="Z4">
-        <v>2.579336690678772</v>
+        <v>2.579296971163119</v>
       </c>
       <c r="AA4">
-        <v>-5.96617270910441E-07</v>
+        <v>-5.966173124008846E-07</v>
       </c>
       <c r="AB4">
-        <v>3.086714267335903</v>
+        <v>3.086666735785285</v>
       </c>
       <c r="AC4">
-        <v>-1.791370492863834E-07</v>
+        <v>-1.791146375175698E-07</v>
       </c>
       <c r="AD4">
-        <v>-1.69530555368151</v>
+        <v>-1.695279449585117</v>
       </c>
       <c r="AE4">
-        <v>-5.915974641907059E-07</v>
+        <v>-5.916188057279711E-07</v>
       </c>
       <c r="AF4">
-        <v>0.323766488310834</v>
+        <v>0.3237615017416037</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -945,7 +945,7 @@
         <v>3.086787105915669</v>
       </c>
       <c r="AC5">
-        <v>-5.406482465462274E-07</v>
+        <v>-5.406482465462275E-07</v>
       </c>
       <c r="AD5">
         <v>-1.69528869996455</v>
@@ -1013,46 +1013,46 @@
         <v>9999.686604517508</v>
       </c>
       <c r="S6">
-        <v>0.0008307886036718343</v>
+        <v>0.0008308706508825413</v>
       </c>
       <c r="T6">
-        <v>-12.99886905684819</v>
+        <v>-12.99846623850372</v>
       </c>
       <c r="U6">
-        <v>-0.000219253777153926</v>
+        <v>-0.0002192530052636901</v>
       </c>
       <c r="V6">
-        <v>0.2777010712261758</v>
+        <v>0.27769713835233</v>
       </c>
       <c r="W6">
-        <v>-4.419338793888598E-05</v>
+        <v>-4.419065289680839E-05</v>
       </c>
       <c r="X6">
-        <v>1.784569123824055</v>
+        <v>1.784511003164041</v>
       </c>
       <c r="Y6">
-        <v>-1.466484580937218E-06</v>
+        <v>-1.466536158456543E-06</v>
       </c>
       <c r="Z6">
-        <v>2.576905122041345</v>
+        <v>2.576825011735771</v>
       </c>
       <c r="AA6">
-        <v>-2.603098273404642E-06</v>
+        <v>-2.60310304880167E-06</v>
       </c>
       <c r="AB6">
-        <v>3.087016991444953</v>
+        <v>3.086920153558611</v>
       </c>
       <c r="AC6">
-        <v>9.1516474039919E-07</v>
+        <v>9.151666291426928E-07</v>
       </c>
       <c r="AD6">
-        <v>-1.695096375684082</v>
+        <v>-1.695043311474559</v>
       </c>
       <c r="AE6">
-        <v>-2.788832556987213E-06</v>
+        <v>-2.788866050663632E-06</v>
       </c>
       <c r="AF6">
-        <v>0.3235517978502203</v>
+        <v>0.3235417131396416</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -1111,46 +1111,46 @@
         <v>3924.583743737668</v>
       </c>
       <c r="S7">
-        <v>-0.2664069153075049</v>
+        <v>-0.001703083995411835</v>
       </c>
       <c r="T7">
-        <v>732.0905336348602</v>
+        <v>-2.912983473620887</v>
       </c>
       <c r="U7">
-        <v>-0.01983842572494893</v>
+        <v>-0.000122347679660836</v>
       </c>
       <c r="V7">
-        <v>357.9478538335806</v>
+        <v>-0.07706840814960061</v>
       </c>
       <c r="W7">
-        <v>0.001331799116434746</v>
+        <v>2.349075611653704E-05</v>
       </c>
       <c r="X7">
-        <v>124.1039117647692</v>
+        <v>-2.024201225339</v>
       </c>
       <c r="Y7">
-        <v>-0.000581540885001387</v>
+        <v>1.976982359299177E-06</v>
       </c>
       <c r="Z7">
-        <v>45.68089166192325</v>
+        <v>-0.4878575412004966</v>
       </c>
       <c r="AA7">
-        <v>-2.131295993674912E-05</v>
+        <v>-1.790028598755125E-07</v>
       </c>
       <c r="AB7">
-        <v>17.56577122913476</v>
+        <v>0.2602097271581776</v>
       </c>
       <c r="AC7">
-        <v>0.0006067413513743717</v>
+        <v>4.500950413440616E-07</v>
       </c>
       <c r="AD7">
-        <v>5.911530117808881</v>
+        <v>-0.5309228916190798</v>
       </c>
       <c r="AE7">
-        <v>0.0003945885488136774</v>
+        <v>2.304550423522201E-06</v>
       </c>
       <c r="AF7">
-        <v>2.44918292339739</v>
+        <v>0.04986165914984727</v>
       </c>
     </row>
     <row r="8" spans="1:32">
@@ -1209,46 +1209,46 @@
         <v>1.629919257347524</v>
       </c>
       <c r="S8">
-        <v>-0.2241967543583217</v>
+        <v>-3.101201890367674E-05</v>
       </c>
       <c r="T8">
-        <v>13.36935793973882</v>
+        <v>0.004891586602117523</v>
       </c>
       <c r="U8">
-        <v>-0.01011433821218637</v>
+        <v>-2.079313957908111E-06</v>
       </c>
       <c r="V8">
-        <v>-0.3463083933613519</v>
+        <v>-2.278909536938637E-05</v>
       </c>
       <c r="W8">
-        <v>0.009535958439886217</v>
+        <v>1.477197993531028E-06</v>
       </c>
       <c r="X8">
-        <v>0.6722488571783672</v>
+        <v>9.616244135084262E-05</v>
       </c>
       <c r="Y8">
-        <v>0.005900677588224554</v>
+        <v>7.749681568662174E-07</v>
       </c>
       <c r="Z8">
-        <v>0.2557707902136752</v>
+        <v>2.836587273695381E-05</v>
       </c>
       <c r="AA8">
-        <v>0.0006709541502853638</v>
+        <v>2.19672190335622E-07</v>
       </c>
       <c r="AB8">
-        <v>0.4136810761555675</v>
+        <v>5.50600451644013E-05</v>
       </c>
       <c r="AC8">
-        <v>-0.008947630803538735</v>
+        <v>-1.315272239759572E-06</v>
       </c>
       <c r="AD8">
-        <v>-1.197859966876656</v>
+        <v>-0.0001700515840499074</v>
       </c>
       <c r="AE8">
-        <v>-0.005015797054788405</v>
+        <v>-8.665636477264422E-07</v>
       </c>
       <c r="AF8">
-        <v>0.5390454768932538</v>
+        <v>6.589463835234729E-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>